<commit_message>
Created function for sample point creation
</commit_message>
<xml_diff>
--- a/v11/XRay/InputOutput/S0001_x_5d_Crash_Problem.xlsx
+++ b/v11/XRay/InputOutput/S0001_x_5d_Crash_Problem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\intern\06_Themen\20_X-Ray_Tool\v11\v11\XRay\InputOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoh\Code\Xray_hoh\v11\XRay\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA0286A-0B23-4298-9981-F4AE2DA52644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2182770-B8A6-4E6E-9003-8AB2144FC5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{691BFE3F-6802-4FDA-8B39-D8BCBE8D77A0}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15285" activeTab="1" xr2:uid="{691BFE3F-6802-4FDA-8B39-D8BCBE8D77A0}"/>
   </bookViews>
   <sheets>
     <sheet name="design_variables" sheetId="2" r:id="rId1"/>
@@ -446,7 +446,7 @@
         <v>437209.30232558155</v>
       </c>
       <c r="C1">
-        <v>637068.35799859045</v>
+        <v>697674.41860465112</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -457,7 +457,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2052.5581395348845</v>
+        <v>1932.558139534884</v>
       </c>
       <c r="C2">
         <v>2500</v>

</xml_diff>

<commit_message>
embedded most recent files from OneDrive
</commit_message>
<xml_diff>
--- a/v11/XRay/InputOutput/S0001_x_5d_Crash_Problem.xlsx
+++ b/v11/XRay/InputOutput/S0001_x_5d_Crash_Problem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoh\Code\Xray_hoh\v11\XRay\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2182770-B8A6-4E6E-9003-8AB2144FC5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C4D291-100D-49CC-AE92-F79110F97F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15285" activeTab="1" xr2:uid="{691BFE3F-6802-4FDA-8B39-D8BCBE8D77A0}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="38700" windowHeight="15285" activeTab="1" xr2:uid="{691BFE3F-6802-4FDA-8B39-D8BCBE8D77A0}"/>
   </bookViews>
   <sheets>
     <sheet name="design_variables" sheetId="2" r:id="rId1"/>
@@ -436,7 +436,7 @@
       <selection activeCell="D1" sqref="D1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -535,7 +535,7 @@
       <selection activeCell="D1" sqref="D1:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>